<commit_message>
adding more info about modules
</commit_message>
<xml_diff>
--- a/esco/csv/modules.xlsx
+++ b/esco/csv/modules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSITA\work\fhnw_maja\code\esco\courses_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSITA\work\fhnw_maja\iModuleBuddy\esco\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5E0ADB-BC19-45C2-B1FA-589427E59F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7130D6C-A3E0-4FA2-9EBB-C1C915446BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{353C9A4D-0E75-460D-8E31-57DD1E737141}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="202">
   <si>
     <t>Individual Name</t>
   </si>
@@ -1235,6 +1235,9 @@
 The 3rd part deals with the transformation of organizations and innovation aspects
 such as Digitalization or AI.
 The final part is elaborating the future based on data universes.</t>
+  </si>
+  <si>
+    <t>ECTS</t>
   </si>
 </sst>
 </file>
@@ -1651,10 +1654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549F31CB-AAAF-459F-92B3-74DB71577A6A}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,7 +1673,7 @@
     <col min="10" max="10" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1701,8 +1704,11 @@
       <c r="J1" s="5" t="s">
         <v>185</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>201</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -1726,8 +1732,11 @@
       <c r="I2" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="K2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -1753,8 +1762,11 @@
       <c r="I3" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>154</v>
       </c>
@@ -1782,8 +1794,11 @@
       <c r="I4" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -1814,8 +1829,11 @@
       <c r="J5" t="s">
         <v>158</v>
       </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -1843,8 +1861,11 @@
       <c r="I6" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="K6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -1868,8 +1889,11 @@
       <c r="I7" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>158</v>
       </c>
@@ -1895,8 +1919,11 @@
       <c r="I8" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>159</v>
       </c>
@@ -1920,8 +1947,11 @@
       <c r="I9" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -1947,8 +1977,11 @@
       <c r="I10" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>161</v>
       </c>
@@ -1976,8 +2009,11 @@
       <c r="I11" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>195</v>
       </c>
@@ -1999,8 +2035,11 @@
       <c r="I12" s="1" t="s">
         <v>200</v>
       </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>162</v>
       </c>
@@ -2026,8 +2065,11 @@
       <c r="I13" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>163</v>
       </c>
@@ -2058,8 +2100,11 @@
       <c r="J14" t="s">
         <v>158</v>
       </c>
+      <c r="K14">
+        <v>6</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>164</v>
       </c>
@@ -2085,8 +2130,11 @@
       <c r="I15" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="K15">
+        <v>6</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>165</v>
       </c>
@@ -2110,8 +2158,11 @@
       <c r="I16" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="K16">
+        <v>6</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>166</v>
       </c>
@@ -2137,8 +2188,11 @@
       <c r="I17" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="K17">
+        <v>6</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>187</v>
       </c>
@@ -2164,8 +2218,11 @@
       <c r="I18" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="K18">
+        <v>6</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>167</v>
       </c>
@@ -2196,8 +2253,11 @@
       <c r="J19" t="s">
         <v>158</v>
       </c>
+      <c r="K19">
+        <v>6</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>168</v>
       </c>
@@ -2223,8 +2283,11 @@
       <c r="I20" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="K20">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>169</v>
       </c>
@@ -2248,8 +2311,11 @@
       <c r="I21" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="K21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>170</v>
       </c>
@@ -2278,8 +2344,11 @@
       <c r="J22" t="s">
         <v>171</v>
       </c>
+      <c r="K22">
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>171</v>
       </c>
@@ -2308,8 +2377,11 @@
       <c r="J23" t="s">
         <v>174</v>
       </c>
+      <c r="K23">
+        <v>6</v>
+      </c>
     </row>
-    <row r="24" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>172</v>
       </c>
@@ -2335,8 +2407,11 @@
       <c r="I24" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="K24">
+        <v>6</v>
+      </c>
     </row>
-    <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>173</v>
       </c>
@@ -2363,7 +2438,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>174</v>
       </c>
@@ -2388,7 +2463,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>175</v>
       </c>
@@ -2415,7 +2490,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>176</v>
       </c>
@@ -2459,12 +2534,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="48d1d936-0e7a-4043-8345-a8484203a87a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="58be894e-647b-4a56-9e0a-41344ee8d54b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2671,20 +2748,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="48d1d936-0e7a-4043-8345-a8484203a87a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="58be894e-647b-4a56-9e0a-41344ee8d54b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FD47E3E-2FF0-47A3-8EDF-48E41399458D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E783A08-661B-4E4C-AF84-8F056E7E9050}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="48d1d936-0e7a-4043-8345-a8484203a87a"/>
+    <ds:schemaRef ds:uri="58be894e-647b-4a56-9e0a-41344ee8d54b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2709,12 +2787,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E783A08-661B-4E4C-AF84-8F056E7E9050}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FD47E3E-2FF0-47A3-8EDF-48E41399458D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="48d1d936-0e7a-4043-8345-a8484203a87a"/>
-    <ds:schemaRef ds:uri="58be894e-647b-4a56-9e0a-41344ee8d54b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>